<commit_message>
Decided to add accessibility
</commit_message>
<xml_diff>
--- a/ana/resilient.xlsx
+++ b/ana/resilient.xlsx
@@ -8,32 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu.6544\Documents\GitHub\COTA-AccessibilityReliability\ana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A622470F-ACF0-4E9A-82F7-E8608DA06225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555EAC65-129E-484B-95F1-DF46294AC3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="date&amp;time" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="football" sheetId="5" r:id="rId3"/>
-    <sheet name="control" sheetId="6" r:id="rId4"/>
-    <sheet name="30 minutes" sheetId="8" r:id="rId5"/>
-    <sheet name="60 minutes" sheetId="9" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="10" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId8"/>
-    <sheet name="Sheet4" sheetId="12" r:id="rId9"/>
-    <sheet name="raw_access_reliab_30min" sheetId="13" r:id="rId10"/>
-    <sheet name="access_reliab_home" sheetId="14" r:id="rId11"/>
-    <sheet name="access_reliab_away" sheetId="20" r:id="rId12"/>
-    <sheet name="access_reliab_normal" sheetId="19" r:id="rId13"/>
-    <sheet name="Sheet8" sheetId="16" r:id="rId14"/>
-    <sheet name="peak_number" sheetId="17" r:id="rId15"/>
-    <sheet name="peak_hour" sheetId="18" r:id="rId16"/>
+    <sheet name="access_access_home" sheetId="22" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="football" sheetId="5" state="hidden" r:id="rId4"/>
+    <sheet name="control" sheetId="6" state="hidden" r:id="rId5"/>
+    <sheet name="30 minutes" sheetId="8" state="hidden" r:id="rId6"/>
+    <sheet name="60 minutes" sheetId="9" state="hidden" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="10" state="hidden" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="11" state="hidden" r:id="rId9"/>
+    <sheet name="Sheet4" sheetId="12" state="hidden" r:id="rId10"/>
+    <sheet name="raw_access_reliab_30min" sheetId="13" state="hidden" r:id="rId11"/>
+    <sheet name="access_reliab_home" sheetId="14" r:id="rId12"/>
+    <sheet name="access_reliab_away" sheetId="20" r:id="rId13"/>
+    <sheet name="access_reliab_normal" sheetId="19" r:id="rId14"/>
+    <sheet name="Sheet8" sheetId="16" state="hidden" r:id="rId15"/>
+    <sheet name="peak_number" sheetId="17" r:id="rId16"/>
+    <sheet name="peak_hour" sheetId="18" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">peak_hour!$A$1:$G$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">peak_number!$A$1:$D$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Sheet8!$A$1:$D$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">peak_hour!$A$1:$G$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">peak_number!$A$1:$D$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Sheet8!$A$1:$D$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24527,6 +24528,1203 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B1A811-A38F-4335-A6D5-4CAA636AF908}">
+  <dimension ref="A1:X16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:X16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>10</v>
+      </c>
+      <c r="D1">
+        <v>15</v>
+      </c>
+      <c r="E1">
+        <v>20</v>
+      </c>
+      <c r="F1">
+        <v>25</v>
+      </c>
+      <c r="G1">
+        <v>30</v>
+      </c>
+      <c r="H1">
+        <v>35</v>
+      </c>
+      <c r="I1">
+        <v>40</v>
+      </c>
+      <c r="J1">
+        <v>45</v>
+      </c>
+      <c r="K1">
+        <v>50</v>
+      </c>
+      <c r="L1">
+        <v>55</v>
+      </c>
+      <c r="M1">
+        <v>60</v>
+      </c>
+      <c r="N1">
+        <v>65</v>
+      </c>
+      <c r="O1">
+        <v>70</v>
+      </c>
+      <c r="P1">
+        <v>75</v>
+      </c>
+      <c r="Q1">
+        <v>80</v>
+      </c>
+      <c r="R1">
+        <v>85</v>
+      </c>
+      <c r="S1">
+        <v>90</v>
+      </c>
+      <c r="T1">
+        <v>95</v>
+      </c>
+      <c r="U1">
+        <v>100</v>
+      </c>
+      <c r="V1">
+        <v>105</v>
+      </c>
+      <c r="W1">
+        <v>110</v>
+      </c>
+      <c r="X1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>0.140725844167991</v>
+      </c>
+      <c r="C2">
+        <v>0.212302973502598</v>
+      </c>
+      <c r="D2">
+        <v>0.272598262664487</v>
+      </c>
+      <c r="E2">
+        <v>0.30479582516741099</v>
+      </c>
+      <c r="F2">
+        <v>0.34253357159967901</v>
+      </c>
+      <c r="G2">
+        <v>0.33930418480368901</v>
+      </c>
+      <c r="H2">
+        <v>0.38916358473037899</v>
+      </c>
+      <c r="I2">
+        <v>0.41153904484168002</v>
+      </c>
+      <c r="J2">
+        <v>0.41542395619811601</v>
+      </c>
+      <c r="K2">
+        <v>0.44649572059598303</v>
+      </c>
+      <c r="L2">
+        <v>0.45180277182537798</v>
+      </c>
+      <c r="M2">
+        <v>0.41449070115732001</v>
+      </c>
+      <c r="N2">
+        <v>0.39794823810114999</v>
+      </c>
+      <c r="O2">
+        <v>0.377327647297236</v>
+      </c>
+      <c r="P2">
+        <v>0.35432417513574699</v>
+      </c>
+      <c r="Q2">
+        <v>0.33712136370013102</v>
+      </c>
+      <c r="R2">
+        <v>0.329311506878532</v>
+      </c>
+      <c r="S2">
+        <v>0.307866107886271</v>
+      </c>
+      <c r="T2">
+        <v>0.28852491954231402</v>
+      </c>
+      <c r="U2">
+        <v>0.26562471516771402</v>
+      </c>
+      <c r="V2">
+        <v>0.24396939171720999</v>
+      </c>
+      <c r="W2">
+        <v>0.236286439777697</v>
+      </c>
+      <c r="X2">
+        <v>0.221827528065869</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>0.14131697569589599</v>
+      </c>
+      <c r="C3">
+        <v>0.20817032422720999</v>
+      </c>
+      <c r="D3">
+        <v>0.27888798377731899</v>
+      </c>
+      <c r="E3">
+        <v>0.33631633227076602</v>
+      </c>
+      <c r="F3">
+        <v>0.38546324692605899</v>
+      </c>
+      <c r="G3">
+        <v>0.38769878840011202</v>
+      </c>
+      <c r="H3">
+        <v>0.413248215302014</v>
+      </c>
+      <c r="I3">
+        <v>0.41100115474411197</v>
+      </c>
+      <c r="J3">
+        <v>0.43128436456631303</v>
+      </c>
+      <c r="K3">
+        <v>0.48877898652658203</v>
+      </c>
+      <c r="L3">
+        <v>0.50939998356440896</v>
+      </c>
+      <c r="M3">
+        <v>0.48818475713342302</v>
+      </c>
+      <c r="N3">
+        <v>0.484804739089778</v>
+      </c>
+      <c r="O3">
+        <v>0.47314007252006601</v>
+      </c>
+      <c r="P3">
+        <v>0.45857433864429797</v>
+      </c>
+      <c r="Q3">
+        <v>0.432059159452931</v>
+      </c>
+      <c r="R3">
+        <v>0.39996515593174797</v>
+      </c>
+      <c r="S3">
+        <v>0.35952088051961001</v>
+      </c>
+      <c r="T3">
+        <v>0.33358436747495201</v>
+      </c>
+      <c r="U3">
+        <v>0.30888273567408697</v>
+      </c>
+      <c r="V3">
+        <v>0.28835487743580202</v>
+      </c>
+      <c r="W3">
+        <v>0.27104563089142403</v>
+      </c>
+      <c r="X3">
+        <v>0.25033045908128898</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>0.13052543786488699</v>
+      </c>
+      <c r="C4">
+        <v>0.19656410951477299</v>
+      </c>
+      <c r="D4">
+        <v>0.30687878189359502</v>
+      </c>
+      <c r="E4">
+        <v>0.36927978745932999</v>
+      </c>
+      <c r="F4">
+        <v>0.37944924730086999</v>
+      </c>
+      <c r="G4">
+        <v>0.35942564312202502</v>
+      </c>
+      <c r="H4">
+        <v>0.41979896697872499</v>
+      </c>
+      <c r="I4">
+        <v>0.43426571761849198</v>
+      </c>
+      <c r="J4">
+        <v>0.43142948486478999</v>
+      </c>
+      <c r="K4">
+        <v>0.463558951841199</v>
+      </c>
+      <c r="L4">
+        <v>0.46235839580413501</v>
+      </c>
+      <c r="M4">
+        <v>0.43392205315356702</v>
+      </c>
+      <c r="N4">
+        <v>0.42900142694499699</v>
+      </c>
+      <c r="O4">
+        <v>0.42742206722127801</v>
+      </c>
+      <c r="P4">
+        <v>0.41441749295846803</v>
+      </c>
+      <c r="Q4">
+        <v>0.38478491112464502</v>
+      </c>
+      <c r="R4">
+        <v>0.360976037914089</v>
+      </c>
+      <c r="S4">
+        <v>0.33342078221223298</v>
+      </c>
+      <c r="T4">
+        <v>0.30483180409069099</v>
+      </c>
+      <c r="U4">
+        <v>0.28455875286571902</v>
+      </c>
+      <c r="V4">
+        <v>0.26385540892439402</v>
+      </c>
+      <c r="W4">
+        <v>0.25145687139359801</v>
+      </c>
+      <c r="X4">
+        <v>0.23575277024008001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0.12864733849165599</v>
+      </c>
+      <c r="C5">
+        <v>0.24846250611503201</v>
+      </c>
+      <c r="D5">
+        <v>0.35474326630555703</v>
+      </c>
+      <c r="E5">
+        <v>0.37337889297882798</v>
+      </c>
+      <c r="F5">
+        <v>0.41114866850861198</v>
+      </c>
+      <c r="G5">
+        <v>0.40940229689756602</v>
+      </c>
+      <c r="H5">
+        <v>0.44525990306093899</v>
+      </c>
+      <c r="I5">
+        <v>0.48060087054404399</v>
+      </c>
+      <c r="J5">
+        <v>0.50544341978658702</v>
+      </c>
+      <c r="K5">
+        <v>0.54779823241094505</v>
+      </c>
+      <c r="L5">
+        <v>0.55146271257894497</v>
+      </c>
+      <c r="M5">
+        <v>0.522730286792503</v>
+      </c>
+      <c r="N5">
+        <v>0.496989448865226</v>
+      </c>
+      <c r="O5">
+        <v>0.480845224041835</v>
+      </c>
+      <c r="P5">
+        <v>0.45727943261614801</v>
+      </c>
+      <c r="Q5">
+        <v>0.426289508811031</v>
+      </c>
+      <c r="R5">
+        <v>0.40951059206265999</v>
+      </c>
+      <c r="S5">
+        <v>0.38278107085539498</v>
+      </c>
+      <c r="T5">
+        <v>0.35700528606952597</v>
+      </c>
+      <c r="U5">
+        <v>0.31832321933532498</v>
+      </c>
+      <c r="V5">
+        <v>0.29438428711319797</v>
+      </c>
+      <c r="W5">
+        <v>0.27563303283559099</v>
+      </c>
+      <c r="X5">
+        <v>0.25406489545389399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>9.0752804922186001E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.21392734608024</v>
+      </c>
+      <c r="D6">
+        <v>0.35851407214451497</v>
+      </c>
+      <c r="E6">
+        <v>0.41562359087587197</v>
+      </c>
+      <c r="F6">
+        <v>0.45983042854927397</v>
+      </c>
+      <c r="G6">
+        <v>0.51327330439852303</v>
+      </c>
+      <c r="H6">
+        <v>0.56432651035171599</v>
+      </c>
+      <c r="I6">
+        <v>0.56289779845679799</v>
+      </c>
+      <c r="J6">
+        <v>0.58452075969704798</v>
+      </c>
+      <c r="K6">
+        <v>0.59141588341530504</v>
+      </c>
+      <c r="L6">
+        <v>0.59761929260859403</v>
+      </c>
+      <c r="M6">
+        <v>0.54986062239295597</v>
+      </c>
+      <c r="N6">
+        <v>0.553662140272563</v>
+      </c>
+      <c r="O6">
+        <v>0.53580561536985905</v>
+      </c>
+      <c r="P6">
+        <v>0.48704822667519199</v>
+      </c>
+      <c r="Q6">
+        <v>0.45029806083803497</v>
+      </c>
+      <c r="R6">
+        <v>0.43521839114732203</v>
+      </c>
+      <c r="S6">
+        <v>0.39829118383609402</v>
+      </c>
+      <c r="T6">
+        <v>0.357235066772851</v>
+      </c>
+      <c r="U6">
+        <v>0.31579591846254601</v>
+      </c>
+      <c r="V6">
+        <v>0.286295858317348</v>
+      </c>
+      <c r="W6">
+        <v>0.26818139993289503</v>
+      </c>
+      <c r="X6">
+        <v>0.25273696695806802</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>0.14879369300911799</v>
+      </c>
+      <c r="C7">
+        <v>0.29907445266327098</v>
+      </c>
+      <c r="D7">
+        <v>0.41457506361323099</v>
+      </c>
+      <c r="E7">
+        <v>0.44969622078055799</v>
+      </c>
+      <c r="F7">
+        <v>0.48309217960540801</v>
+      </c>
+      <c r="G7">
+        <v>0.461559065531644</v>
+      </c>
+      <c r="H7">
+        <v>0.51031859786015399</v>
+      </c>
+      <c r="I7">
+        <v>0.52296974128686102</v>
+      </c>
+      <c r="J7">
+        <v>0.54379386955306197</v>
+      </c>
+      <c r="K7">
+        <v>0.59001005788101102</v>
+      </c>
+      <c r="L7">
+        <v>0.59556008287816398</v>
+      </c>
+      <c r="M7">
+        <v>0.56976231126952404</v>
+      </c>
+      <c r="N7">
+        <v>0.54968926796902295</v>
+      </c>
+      <c r="O7">
+        <v>0.52159005853989904</v>
+      </c>
+      <c r="P7">
+        <v>0.50248184591143097</v>
+      </c>
+      <c r="Q7">
+        <v>0.4696102378973</v>
+      </c>
+      <c r="R7">
+        <v>0.46189632610766201</v>
+      </c>
+      <c r="S7">
+        <v>0.42794194233229099</v>
+      </c>
+      <c r="T7">
+        <v>0.39433530684426099</v>
+      </c>
+      <c r="U7">
+        <v>0.35732273671577403</v>
+      </c>
+      <c r="V7">
+        <v>0.32298956931045703</v>
+      </c>
+      <c r="W7">
+        <v>0.29953765941858801</v>
+      </c>
+      <c r="X7">
+        <v>0.279596310347276</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>0.13379690125070001</v>
+      </c>
+      <c r="C8">
+        <v>0.25905816388090402</v>
+      </c>
+      <c r="D8">
+        <v>0.39949400463344398</v>
+      </c>
+      <c r="E8">
+        <v>0.45745816640415998</v>
+      </c>
+      <c r="F8">
+        <v>0.46465964060864501</v>
+      </c>
+      <c r="G8">
+        <v>0.45991806398539697</v>
+      </c>
+      <c r="H8">
+        <v>0.48214861230345302</v>
+      </c>
+      <c r="I8">
+        <v>0.49676184578426902</v>
+      </c>
+      <c r="J8">
+        <v>0.49193614800185997</v>
+      </c>
+      <c r="K8">
+        <v>0.50279462966055</v>
+      </c>
+      <c r="L8">
+        <v>0.51791941381598405</v>
+      </c>
+      <c r="M8">
+        <v>0.47443264776543298</v>
+      </c>
+      <c r="N8">
+        <v>0.45377076440218</v>
+      </c>
+      <c r="O8">
+        <v>0.42579853209773599</v>
+      </c>
+      <c r="P8">
+        <v>0.40729591318403402</v>
+      </c>
+      <c r="Q8">
+        <v>0.36732145710453901</v>
+      </c>
+      <c r="R8">
+        <v>0.36000065854280899</v>
+      </c>
+      <c r="S8">
+        <v>0.33176274553083401</v>
+      </c>
+      <c r="T8">
+        <v>0.29563291098519101</v>
+      </c>
+      <c r="U8">
+        <v>0.25939272919395201</v>
+      </c>
+      <c r="V8">
+        <v>0.23604149140681599</v>
+      </c>
+      <c r="W8">
+        <v>0.21734477090837701</v>
+      </c>
+      <c r="X8">
+        <v>0.204199209921752</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>0.124647203072225</v>
+      </c>
+      <c r="C9">
+        <v>0.214850166865521</v>
+      </c>
+      <c r="D9">
+        <v>0.30632070045376097</v>
+      </c>
+      <c r="E9">
+        <v>0.35415738788760498</v>
+      </c>
+      <c r="F9">
+        <v>0.37172068883887999</v>
+      </c>
+      <c r="G9">
+        <v>0.35110170793412498</v>
+      </c>
+      <c r="H9">
+        <v>0.38993219283243802</v>
+      </c>
+      <c r="I9">
+        <v>0.40950334502225799</v>
+      </c>
+      <c r="J9">
+        <v>0.43161126151095403</v>
+      </c>
+      <c r="K9">
+        <v>0.44474389773003498</v>
+      </c>
+      <c r="L9">
+        <v>0.45315682634590898</v>
+      </c>
+      <c r="M9">
+        <v>0.437114215847974</v>
+      </c>
+      <c r="N9">
+        <v>0.431013380693758</v>
+      </c>
+      <c r="O9">
+        <v>0.417511169654811</v>
+      </c>
+      <c r="P9">
+        <v>0.39593724974019101</v>
+      </c>
+      <c r="Q9">
+        <v>0.37705356525880901</v>
+      </c>
+      <c r="R9">
+        <v>0.368745595241946</v>
+      </c>
+      <c r="S9">
+        <v>0.34968190525641202</v>
+      </c>
+      <c r="T9">
+        <v>0.327756606332051</v>
+      </c>
+      <c r="U9">
+        <v>0.30336549266139801</v>
+      </c>
+      <c r="V9">
+        <v>0.28552353892535398</v>
+      </c>
+      <c r="W9">
+        <v>0.26608755168501502</v>
+      </c>
+      <c r="X9">
+        <v>0.24595549675496101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>0.118118628359592</v>
+      </c>
+      <c r="C10">
+        <v>0.21693149531726799</v>
+      </c>
+      <c r="D10">
+        <v>0.29992041639605099</v>
+      </c>
+      <c r="E10">
+        <v>0.35233139963718202</v>
+      </c>
+      <c r="F10">
+        <v>0.38290810471254699</v>
+      </c>
+      <c r="G10">
+        <v>0.40671670803552701</v>
+      </c>
+      <c r="H10">
+        <v>0.45835177077716099</v>
+      </c>
+      <c r="I10">
+        <v>0.47130450335037199</v>
+      </c>
+      <c r="J10">
+        <v>0.48322476097109701</v>
+      </c>
+      <c r="K10">
+        <v>0.49913512470862897</v>
+      </c>
+      <c r="L10">
+        <v>0.51318161594704204</v>
+      </c>
+      <c r="M10">
+        <v>0.50166270414743597</v>
+      </c>
+      <c r="N10">
+        <v>0.49406051720008198</v>
+      </c>
+      <c r="O10">
+        <v>0.48126485949013798</v>
+      </c>
+      <c r="P10">
+        <v>0.448208601359672</v>
+      </c>
+      <c r="Q10">
+        <v>0.41346020822432999</v>
+      </c>
+      <c r="R10">
+        <v>0.40669196936798901</v>
+      </c>
+      <c r="S10">
+        <v>0.38858369153864403</v>
+      </c>
+      <c r="T10">
+        <v>0.36719345875529502</v>
+      </c>
+      <c r="U10">
+        <v>0.33775153968337601</v>
+      </c>
+      <c r="V10">
+        <v>0.30901792511592402</v>
+      </c>
+      <c r="W10">
+        <v>0.28732630409541299</v>
+      </c>
+      <c r="X10">
+        <v>0.27227040227252203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>0.10914508365803301</v>
+      </c>
+      <c r="C11">
+        <v>0.21328410725737901</v>
+      </c>
+      <c r="D11">
+        <v>0.28233604165731402</v>
+      </c>
+      <c r="E11">
+        <v>0.31554864762790102</v>
+      </c>
+      <c r="F11">
+        <v>0.35032310296607</v>
+      </c>
+      <c r="G11">
+        <v>0.34270727923467798</v>
+      </c>
+      <c r="H11">
+        <v>0.388267528414939</v>
+      </c>
+      <c r="I11">
+        <v>0.42467138828406797</v>
+      </c>
+      <c r="J11">
+        <v>0.43290888526667498</v>
+      </c>
+      <c r="K11">
+        <v>0.44459822553192202</v>
+      </c>
+      <c r="L11">
+        <v>0.45724306588180302</v>
+      </c>
+      <c r="M11">
+        <v>0.45965578738273699</v>
+      </c>
+      <c r="N11">
+        <v>0.43990694723485202</v>
+      </c>
+      <c r="O11">
+        <v>0.41230060067091201</v>
+      </c>
+      <c r="P11">
+        <v>0.38157988668385401</v>
+      </c>
+      <c r="Q11">
+        <v>0.35460810786786701</v>
+      </c>
+      <c r="R11">
+        <v>0.33926144322443602</v>
+      </c>
+      <c r="S11">
+        <v>0.321264220720475</v>
+      </c>
+      <c r="T11">
+        <v>0.304215986126808</v>
+      </c>
+      <c r="U11">
+        <v>0.28399275586109701</v>
+      </c>
+      <c r="V11">
+        <v>0.25740834989614803</v>
+      </c>
+      <c r="W11">
+        <v>0.24404128331428199</v>
+      </c>
+      <c r="X11">
+        <v>0.23071010281500501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>0.119079587017917</v>
+      </c>
+      <c r="C12">
+        <v>0.22936052094062601</v>
+      </c>
+      <c r="D12">
+        <v>0.30951443099620402</v>
+      </c>
+      <c r="E12">
+        <v>0.37799876257384601</v>
+      </c>
+      <c r="F12">
+        <v>0.376261293058958</v>
+      </c>
+      <c r="G12">
+        <v>0.39224322252504101</v>
+      </c>
+      <c r="H12">
+        <v>0.438485072147695</v>
+      </c>
+      <c r="I12">
+        <v>0.45860428951742599</v>
+      </c>
+      <c r="J12">
+        <v>0.481395015255071</v>
+      </c>
+      <c r="K12">
+        <v>0.54322361430223698</v>
+      </c>
+      <c r="L12">
+        <v>0.58157074921859597</v>
+      </c>
+      <c r="M12">
+        <v>0.58834691124570704</v>
+      </c>
+      <c r="N12">
+        <v>0.56076295184508795</v>
+      </c>
+      <c r="O12">
+        <v>0.54126476175885196</v>
+      </c>
+      <c r="P12">
+        <v>0.51852648821539205</v>
+      </c>
+      <c r="Q12">
+        <v>0.495316422925416</v>
+      </c>
+      <c r="R12">
+        <v>0.47991602682080597</v>
+      </c>
+      <c r="S12">
+        <v>0.45229585998628602</v>
+      </c>
+      <c r="T12">
+        <v>0.42559761535458501</v>
+      </c>
+      <c r="U12">
+        <v>0.39765736537795598</v>
+      </c>
+      <c r="V12">
+        <v>0.37666748367104202</v>
+      </c>
+      <c r="W12">
+        <v>0.34776146430409099</v>
+      </c>
+      <c r="X12">
+        <v>0.31928974343370098</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>0.13999245069359201</v>
+      </c>
+      <c r="C13">
+        <v>0.27804790203493601</v>
+      </c>
+      <c r="D13">
+        <v>0.41648770947578301</v>
+      </c>
+      <c r="E13">
+        <v>0.49816124021177399</v>
+      </c>
+      <c r="F13">
+        <v>0.54195853675794203</v>
+      </c>
+      <c r="G13">
+        <v>0.52757047441209304</v>
+      </c>
+      <c r="H13">
+        <v>0.55860703484472196</v>
+      </c>
+      <c r="I13">
+        <v>0.60489072417654599</v>
+      </c>
+      <c r="J13">
+        <v>0.62502855677744695</v>
+      </c>
+      <c r="K13">
+        <v>0.64361679124924798</v>
+      </c>
+      <c r="L13">
+        <v>0.67052032404554796</v>
+      </c>
+      <c r="M13">
+        <v>0.66113544459001805</v>
+      </c>
+      <c r="N13">
+        <v>0.66771959912149503</v>
+      </c>
+      <c r="O13">
+        <v>0.66371940652919503</v>
+      </c>
+      <c r="P13">
+        <v>0.62664089155969604</v>
+      </c>
+      <c r="Q13">
+        <v>0.58011769203608199</v>
+      </c>
+      <c r="R13">
+        <v>0.53687067964981205</v>
+      </c>
+      <c r="S13">
+        <v>0.49171179320944902</v>
+      </c>
+      <c r="T13">
+        <v>0.43877968654559302</v>
+      </c>
+      <c r="U13">
+        <v>0.38615580376413799</v>
+      </c>
+      <c r="V13">
+        <v>0.338803399671121</v>
+      </c>
+      <c r="W13">
+        <v>0.30405087182381801</v>
+      </c>
+      <c r="X13">
+        <v>0.269312158912976</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>0.14984939759036101</v>
+      </c>
+      <c r="C14">
+        <v>0.322312523088289</v>
+      </c>
+      <c r="D14">
+        <v>0.55106145717174004</v>
+      </c>
+      <c r="E14">
+        <v>0.59659477355637602</v>
+      </c>
+      <c r="F14">
+        <v>0.61888611210281996</v>
+      </c>
+      <c r="G14">
+        <v>0.56883739529671895</v>
+      </c>
+      <c r="H14">
+        <v>0.58054739750251905</v>
+      </c>
+      <c r="I14">
+        <v>0.61745042616581702</v>
+      </c>
+      <c r="J14">
+        <v>0.63432475998438997</v>
+      </c>
+      <c r="K14">
+        <v>0.66346800862111099</v>
+      </c>
+      <c r="L14">
+        <v>0.69212337924781198</v>
+      </c>
+      <c r="M14">
+        <v>0.68674382453738003</v>
+      </c>
+      <c r="N14">
+        <v>0.68075908401072405</v>
+      </c>
+      <c r="O14">
+        <v>0.65734374442076304</v>
+      </c>
+      <c r="P14">
+        <v>0.62141264163852195</v>
+      </c>
+      <c r="Q14">
+        <v>0.57939985529323201</v>
+      </c>
+      <c r="R14">
+        <v>0.55379366977975897</v>
+      </c>
+      <c r="S14">
+        <v>0.52080201088586997</v>
+      </c>
+      <c r="T14">
+        <v>0.48230120228182999</v>
+      </c>
+      <c r="U14">
+        <v>0.437403312616024</v>
+      </c>
+      <c r="V14">
+        <v>0.39387206905152999</v>
+      </c>
+      <c r="W14">
+        <v>0.36553843447265599</v>
+      </c>
+      <c r="X14">
+        <v>0.32159028050715399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>0.121665707157935</v>
+      </c>
+      <c r="C15">
+        <v>0.22660089282364801</v>
+      </c>
+      <c r="D15">
+        <v>0.36047685743135399</v>
+      </c>
+      <c r="E15">
+        <v>0.46741026490687299</v>
+      </c>
+      <c r="F15">
+        <v>0.51143095254183801</v>
+      </c>
+      <c r="G15">
+        <v>0.51685134344925998</v>
+      </c>
+      <c r="H15">
+        <v>0.53521973476654605</v>
+      </c>
+      <c r="I15">
+        <v>0.55529910480636302</v>
+      </c>
+      <c r="J15">
+        <v>0.53539335640265395</v>
+      </c>
+      <c r="K15">
+        <v>0.55205958002778299</v>
+      </c>
+      <c r="L15">
+        <v>0.54185046518918001</v>
+      </c>
+      <c r="M15">
+        <v>0.53687402343851798</v>
+      </c>
+      <c r="N15">
+        <v>0.54690083367748998</v>
+      </c>
+      <c r="O15">
+        <v>0.54191467179571595</v>
+      </c>
+      <c r="P15">
+        <v>0.519905705200571</v>
+      </c>
+      <c r="Q15">
+        <v>0.51353863396305</v>
+      </c>
+      <c r="R15">
+        <v>0.53082392874327</v>
+      </c>
+      <c r="S15">
+        <v>0.502136808206881</v>
+      </c>
+      <c r="T15">
+        <v>0.50401674794915696</v>
+      </c>
+      <c r="U15">
+        <v>0.49087591744575299</v>
+      </c>
+      <c r="V15">
+        <v>0.46277702157567202</v>
+      </c>
+      <c r="W15">
+        <v>0.44898297884332899</v>
+      </c>
+      <c r="X15">
+        <v>0.42748525840857599</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>7.9015103686076393E-2</v>
+      </c>
+      <c r="C16">
+        <v>0.15952376204056301</v>
+      </c>
+      <c r="D16">
+        <v>0.243544002718314</v>
+      </c>
+      <c r="E16">
+        <v>0.303172908985057</v>
+      </c>
+      <c r="F16">
+        <v>0.38112126886220898</v>
+      </c>
+      <c r="G16">
+        <v>0.34029427466577</v>
+      </c>
+      <c r="H16">
+        <v>0.396014545572347</v>
+      </c>
+      <c r="I16">
+        <v>0.437818262091349</v>
+      </c>
+      <c r="J16">
+        <v>0.460538177905292</v>
+      </c>
+      <c r="K16">
+        <v>0.49049991772370599</v>
+      </c>
+      <c r="L16">
+        <v>0.47195960881843402</v>
+      </c>
+      <c r="M16">
+        <v>0.45815209510234001</v>
+      </c>
+      <c r="N16">
+        <v>0.474015986704446</v>
+      </c>
+      <c r="O16">
+        <v>0.48624211694706498</v>
+      </c>
+      <c r="P16">
+        <v>0.49889641071583302</v>
+      </c>
+      <c r="Q16">
+        <v>0.51790871561978202</v>
+      </c>
+      <c r="R16">
+        <v>0.54773340072744203</v>
+      </c>
+      <c r="S16">
+        <v>0.53569552514948005</v>
+      </c>
+      <c r="T16">
+        <v>0.57072151652260705</v>
+      </c>
+      <c r="U16">
+        <v>0.59516043468475699</v>
+      </c>
+      <c r="V16">
+        <v>0.58147773609689102</v>
+      </c>
+      <c r="W16">
+        <v>0.56041075340945601</v>
+      </c>
+      <c r="X16">
+        <v>0.53511328224474397</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FAC646-30C9-474D-90F5-9CEA76215738}">
   <dimension ref="A1:P30"/>
   <sheetViews>
@@ -25358,12 +26556,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97EC4F49-7FB8-4751-807F-3492689DAFAE}">
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="B1" sqref="B1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26597,7 +27795,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05EBA4F-6466-4CB8-A00A-33172ED87E46}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -26609,11 +27807,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1172EF6C-D4A3-4EB6-8D73-298C079FEF54}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1:L16"/>
     </sheetView>
   </sheetViews>
@@ -27205,7 +28403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE4E835-AB81-464D-B44F-2B6F511EEA8B}">
   <dimension ref="A1:I28"/>
   <sheetViews>
@@ -27474,7 +28672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8DCF7E-5586-4454-9918-6D1E175C9441}">
   <dimension ref="A1:O19"/>
   <sheetViews>
@@ -27862,7 +29060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D9AB40-23B8-4ECA-8B71-56D8E4D8804A}">
   <dimension ref="A1:H33"/>
   <sheetViews>
@@ -28335,6 +29533,1484 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6716C683-B680-4781-9660-8CD99C8C0C85}">
+  <dimension ref="A1:P30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>8</v>
+      </c>
+      <c r="C1">
+        <v>9</v>
+      </c>
+      <c r="D1">
+        <v>10</v>
+      </c>
+      <c r="E1">
+        <v>11</v>
+      </c>
+      <c r="F1">
+        <v>12</v>
+      </c>
+      <c r="G1">
+        <v>13</v>
+      </c>
+      <c r="H1">
+        <v>14</v>
+      </c>
+      <c r="I1">
+        <v>15</v>
+      </c>
+      <c r="J1">
+        <v>16</v>
+      </c>
+      <c r="K1">
+        <v>17</v>
+      </c>
+      <c r="L1">
+        <v>18</v>
+      </c>
+      <c r="M1">
+        <v>19</v>
+      </c>
+      <c r="N1">
+        <v>20</v>
+      </c>
+      <c r="O1">
+        <v>21</v>
+      </c>
+      <c r="P1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43344</v>
+      </c>
+      <c r="B2">
+        <v>734424</v>
+      </c>
+      <c r="C2">
+        <v>748195</v>
+      </c>
+      <c r="D2">
+        <v>748341</v>
+      </c>
+      <c r="E2">
+        <v>727164</v>
+      </c>
+      <c r="F2">
+        <v>712548</v>
+      </c>
+      <c r="G2">
+        <v>706433</v>
+      </c>
+      <c r="H2">
+        <v>711655</v>
+      </c>
+      <c r="I2">
+        <v>707382</v>
+      </c>
+      <c r="J2">
+        <v>701148</v>
+      </c>
+      <c r="K2">
+        <v>702464</v>
+      </c>
+      <c r="L2">
+        <v>702917</v>
+      </c>
+      <c r="M2">
+        <v>732197</v>
+      </c>
+      <c r="N2">
+        <v>743256</v>
+      </c>
+      <c r="O2">
+        <v>618019</v>
+      </c>
+      <c r="P2">
+        <v>461000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43351</v>
+      </c>
+      <c r="B3">
+        <v>745821</v>
+      </c>
+      <c r="C3">
+        <v>737258</v>
+      </c>
+      <c r="D3">
+        <v>744900</v>
+      </c>
+      <c r="E3">
+        <v>729952</v>
+      </c>
+      <c r="F3">
+        <v>700812</v>
+      </c>
+      <c r="G3">
+        <v>698444</v>
+      </c>
+      <c r="H3">
+        <v>713424</v>
+      </c>
+      <c r="I3">
+        <v>694800</v>
+      </c>
+      <c r="J3">
+        <v>705588</v>
+      </c>
+      <c r="K3">
+        <v>701915</v>
+      </c>
+      <c r="L3">
+        <v>706498</v>
+      </c>
+      <c r="M3">
+        <v>728894</v>
+      </c>
+      <c r="N3">
+        <v>733637</v>
+      </c>
+      <c r="O3">
+        <v>612183</v>
+      </c>
+      <c r="P3">
+        <v>474495</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43365</v>
+      </c>
+      <c r="B4">
+        <v>735308</v>
+      </c>
+      <c r="C4">
+        <v>754907</v>
+      </c>
+      <c r="D4">
+        <v>738290</v>
+      </c>
+      <c r="E4">
+        <v>610229</v>
+      </c>
+      <c r="F4">
+        <v>708759</v>
+      </c>
+      <c r="G4">
+        <v>711519</v>
+      </c>
+      <c r="H4">
+        <v>708948</v>
+      </c>
+      <c r="I4">
+        <v>712128</v>
+      </c>
+      <c r="J4">
+        <v>697964</v>
+      </c>
+      <c r="K4">
+        <v>705969</v>
+      </c>
+      <c r="L4">
+        <v>720668</v>
+      </c>
+      <c r="M4">
+        <v>734747</v>
+      </c>
+      <c r="N4">
+        <v>742033</v>
+      </c>
+      <c r="O4">
+        <v>619070</v>
+      </c>
+      <c r="P4">
+        <v>474236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43379</v>
+      </c>
+      <c r="B5">
+        <v>739831</v>
+      </c>
+      <c r="C5">
+        <v>749611</v>
+      </c>
+      <c r="D5">
+        <v>738011</v>
+      </c>
+      <c r="E5">
+        <v>727950</v>
+      </c>
+      <c r="F5">
+        <v>708501</v>
+      </c>
+      <c r="G5">
+        <v>706039</v>
+      </c>
+      <c r="H5">
+        <v>706422</v>
+      </c>
+      <c r="I5">
+        <v>690378</v>
+      </c>
+      <c r="J5">
+        <v>704943</v>
+      </c>
+      <c r="K5">
+        <v>686347</v>
+      </c>
+      <c r="L5">
+        <v>702341</v>
+      </c>
+      <c r="M5">
+        <v>722324</v>
+      </c>
+      <c r="N5">
+        <v>732866</v>
+      </c>
+      <c r="O5">
+        <v>604694</v>
+      </c>
+      <c r="P5">
+        <v>455077</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43386</v>
+      </c>
+      <c r="B6">
+        <v>737945</v>
+      </c>
+      <c r="C6">
+        <v>749852</v>
+      </c>
+      <c r="D6">
+        <v>745361</v>
+      </c>
+      <c r="E6">
+        <v>728041</v>
+      </c>
+      <c r="F6">
+        <v>706700</v>
+      </c>
+      <c r="G6">
+        <v>702329</v>
+      </c>
+      <c r="H6">
+        <v>705933</v>
+      </c>
+      <c r="I6">
+        <v>703026</v>
+      </c>
+      <c r="J6">
+        <v>697505</v>
+      </c>
+      <c r="K6">
+        <v>676278</v>
+      </c>
+      <c r="L6">
+        <v>711002</v>
+      </c>
+      <c r="M6">
+        <v>718661</v>
+      </c>
+      <c r="N6">
+        <v>724460</v>
+      </c>
+      <c r="O6">
+        <v>607144</v>
+      </c>
+      <c r="P6">
+        <v>465476</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43407</v>
+      </c>
+      <c r="B7">
+        <v>745355</v>
+      </c>
+      <c r="C7">
+        <v>754119</v>
+      </c>
+      <c r="D7">
+        <v>746997</v>
+      </c>
+      <c r="E7">
+        <v>733993</v>
+      </c>
+      <c r="F7">
+        <v>712030</v>
+      </c>
+      <c r="G7">
+        <v>707204</v>
+      </c>
+      <c r="H7">
+        <v>707444</v>
+      </c>
+      <c r="I7">
+        <v>704673</v>
+      </c>
+      <c r="J7">
+        <v>699100</v>
+      </c>
+      <c r="K7">
+        <v>692209</v>
+      </c>
+      <c r="L7">
+        <v>713111</v>
+      </c>
+      <c r="M7">
+        <v>726461</v>
+      </c>
+      <c r="N7">
+        <v>731648</v>
+      </c>
+      <c r="O7">
+        <v>602289</v>
+      </c>
+      <c r="P7">
+        <v>474669</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43428</v>
+      </c>
+      <c r="B8">
+        <v>743167</v>
+      </c>
+      <c r="C8">
+        <v>750316</v>
+      </c>
+      <c r="D8">
+        <v>745081</v>
+      </c>
+      <c r="E8">
+        <v>724445</v>
+      </c>
+      <c r="F8">
+        <v>713362</v>
+      </c>
+      <c r="G8">
+        <v>708524</v>
+      </c>
+      <c r="H8">
+        <v>701135</v>
+      </c>
+      <c r="I8">
+        <v>690956</v>
+      </c>
+      <c r="J8">
+        <v>694351</v>
+      </c>
+      <c r="K8">
+        <v>702972</v>
+      </c>
+      <c r="L8">
+        <v>716611</v>
+      </c>
+      <c r="M8">
+        <v>728579</v>
+      </c>
+      <c r="N8">
+        <v>729400</v>
+      </c>
+      <c r="O8">
+        <v>595884</v>
+      </c>
+      <c r="P8">
+        <v>474358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43715</v>
+      </c>
+      <c r="B9">
+        <v>618525</v>
+      </c>
+      <c r="C9">
+        <v>636566</v>
+      </c>
+      <c r="D9">
+        <v>641578</v>
+      </c>
+      <c r="E9">
+        <v>636890</v>
+      </c>
+      <c r="F9">
+        <v>616119</v>
+      </c>
+      <c r="G9">
+        <v>630959</v>
+      </c>
+      <c r="H9">
+        <v>663526</v>
+      </c>
+      <c r="I9">
+        <v>658664</v>
+      </c>
+      <c r="J9">
+        <v>660256</v>
+      </c>
+      <c r="K9">
+        <v>668391</v>
+      </c>
+      <c r="L9">
+        <v>663992</v>
+      </c>
+      <c r="M9">
+        <v>677412</v>
+      </c>
+      <c r="N9">
+        <v>697709</v>
+      </c>
+      <c r="O9">
+        <v>564384</v>
+      </c>
+      <c r="P9">
+        <v>447775</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43729</v>
+      </c>
+      <c r="B10">
+        <v>612189</v>
+      </c>
+      <c r="C10">
+        <v>631076</v>
+      </c>
+      <c r="D10">
+        <v>659302</v>
+      </c>
+      <c r="E10">
+        <v>621485</v>
+      </c>
+      <c r="F10">
+        <v>604105</v>
+      </c>
+      <c r="G10">
+        <v>592091</v>
+      </c>
+      <c r="H10">
+        <v>620901</v>
+      </c>
+      <c r="I10">
+        <v>618413</v>
+      </c>
+      <c r="J10">
+        <v>601815</v>
+      </c>
+      <c r="K10">
+        <v>615135</v>
+      </c>
+      <c r="L10">
+        <v>646346</v>
+      </c>
+      <c r="M10">
+        <v>639032</v>
+      </c>
+      <c r="N10">
+        <v>618602</v>
+      </c>
+      <c r="O10">
+        <v>480844</v>
+      </c>
+      <c r="P10">
+        <v>415250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43743</v>
+      </c>
+      <c r="B11">
+        <v>718738</v>
+      </c>
+      <c r="C11">
+        <v>706336</v>
+      </c>
+      <c r="D11">
+        <v>694036</v>
+      </c>
+      <c r="E11">
+        <v>697998</v>
+      </c>
+      <c r="F11">
+        <v>676276</v>
+      </c>
+      <c r="G11">
+        <v>676478</v>
+      </c>
+      <c r="H11">
+        <v>670168</v>
+      </c>
+      <c r="I11">
+        <v>669280</v>
+      </c>
+      <c r="J11">
+        <v>667431</v>
+      </c>
+      <c r="K11">
+        <v>653325</v>
+      </c>
+      <c r="L11">
+        <v>685900</v>
+      </c>
+      <c r="M11">
+        <v>688904</v>
+      </c>
+      <c r="N11">
+        <v>710254</v>
+      </c>
+      <c r="O11">
+        <v>573136</v>
+      </c>
+      <c r="P11">
+        <v>439201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43764</v>
+      </c>
+      <c r="B12">
+        <v>535948</v>
+      </c>
+      <c r="C12">
+        <v>491821</v>
+      </c>
+      <c r="D12">
+        <v>543421</v>
+      </c>
+      <c r="E12">
+        <v>340681</v>
+      </c>
+      <c r="F12">
+        <v>552117</v>
+      </c>
+      <c r="G12">
+        <v>596263</v>
+      </c>
+      <c r="H12">
+        <v>639743</v>
+      </c>
+      <c r="I12">
+        <v>606887</v>
+      </c>
+      <c r="J12">
+        <v>650959</v>
+      </c>
+      <c r="K12">
+        <v>671730</v>
+      </c>
+      <c r="L12">
+        <v>673839</v>
+      </c>
+      <c r="M12">
+        <v>690619</v>
+      </c>
+      <c r="N12">
+        <v>685405</v>
+      </c>
+      <c r="O12">
+        <v>580259</v>
+      </c>
+      <c r="P12">
+        <v>433940</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43778</v>
+      </c>
+      <c r="B13">
+        <v>581612</v>
+      </c>
+      <c r="C13">
+        <v>614654</v>
+      </c>
+      <c r="D13">
+        <v>576544</v>
+      </c>
+      <c r="E13">
+        <v>589176</v>
+      </c>
+      <c r="F13">
+        <v>565065</v>
+      </c>
+      <c r="G13">
+        <v>579465</v>
+      </c>
+      <c r="H13">
+        <v>581291</v>
+      </c>
+      <c r="I13">
+        <v>577625</v>
+      </c>
+      <c r="J13">
+        <v>598258</v>
+      </c>
+      <c r="K13">
+        <v>600650</v>
+      </c>
+      <c r="L13">
+        <v>609839</v>
+      </c>
+      <c r="M13">
+        <v>632055</v>
+      </c>
+      <c r="N13">
+        <v>649665</v>
+      </c>
+      <c r="O13">
+        <v>536888</v>
+      </c>
+      <c r="P13">
+        <v>405858</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43792</v>
+      </c>
+      <c r="B14">
+        <v>617017</v>
+      </c>
+      <c r="C14">
+        <v>620832</v>
+      </c>
+      <c r="D14">
+        <v>603596</v>
+      </c>
+      <c r="E14">
+        <v>637160</v>
+      </c>
+      <c r="F14">
+        <v>625778</v>
+      </c>
+      <c r="G14">
+        <v>650931</v>
+      </c>
+      <c r="H14">
+        <v>658690</v>
+      </c>
+      <c r="I14">
+        <v>669415</v>
+      </c>
+      <c r="J14">
+        <v>673573</v>
+      </c>
+      <c r="K14">
+        <v>650741</v>
+      </c>
+      <c r="L14">
+        <v>658404</v>
+      </c>
+      <c r="M14">
+        <v>671206</v>
+      </c>
+      <c r="N14">
+        <v>692721</v>
+      </c>
+      <c r="O14">
+        <v>574142</v>
+      </c>
+      <c r="P14">
+        <v>430732</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15">
+        <f>SUM(B2:B14)</f>
+        <v>8865880</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:P15" si="0">SUM(C2:C14)</f>
+        <v>8945543</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>8925458</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>8505164</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>8602172</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>8666679</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>8789280</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>8703627</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>8752891</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>8728126</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>8911468</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>9091091</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>9191656</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>7568936</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>5852067</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>13</v>
+      </c>
+      <c r="H17">
+        <v>14</v>
+      </c>
+      <c r="I17">
+        <v>15</v>
+      </c>
+      <c r="J17">
+        <v>16</v>
+      </c>
+      <c r="K17">
+        <v>17</v>
+      </c>
+      <c r="L17">
+        <v>18</v>
+      </c>
+      <c r="M17">
+        <v>19</v>
+      </c>
+      <c r="N17">
+        <v>20</v>
+      </c>
+      <c r="O17">
+        <v>21</v>
+      </c>
+      <c r="P17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43344</v>
+      </c>
+      <c r="B18">
+        <v>548158</v>
+      </c>
+      <c r="C18">
+        <v>528306</v>
+      </c>
+      <c r="D18">
+        <v>484302</v>
+      </c>
+      <c r="E18">
+        <v>491549</v>
+      </c>
+      <c r="F18">
+        <v>490734</v>
+      </c>
+      <c r="G18">
+        <v>486767</v>
+      </c>
+      <c r="H18">
+        <v>510283</v>
+      </c>
+      <c r="I18">
+        <v>472250</v>
+      </c>
+      <c r="J18">
+        <v>469800</v>
+      </c>
+      <c r="K18">
+        <v>419661</v>
+      </c>
+      <c r="L18">
+        <v>406022</v>
+      </c>
+      <c r="M18">
+        <v>485309</v>
+      </c>
+      <c r="N18">
+        <v>504349</v>
+      </c>
+      <c r="O18">
+        <v>436393</v>
+      </c>
+      <c r="P18">
+        <v>341779</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43351</v>
+      </c>
+      <c r="B19">
+        <v>556872</v>
+      </c>
+      <c r="C19">
+        <v>531281</v>
+      </c>
+      <c r="D19">
+        <v>547952</v>
+      </c>
+      <c r="E19">
+        <v>517916</v>
+      </c>
+      <c r="F19">
+        <v>463110</v>
+      </c>
+      <c r="G19">
+        <v>477876</v>
+      </c>
+      <c r="H19">
+        <v>488674</v>
+      </c>
+      <c r="I19">
+        <v>514247</v>
+      </c>
+      <c r="J19">
+        <v>501585</v>
+      </c>
+      <c r="K19">
+        <v>522761</v>
+      </c>
+      <c r="L19">
+        <v>507453</v>
+      </c>
+      <c r="M19">
+        <v>477159</v>
+      </c>
+      <c r="N19">
+        <v>467631</v>
+      </c>
+      <c r="O19">
+        <v>403588</v>
+      </c>
+      <c r="P19">
+        <v>354023</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43365</v>
+      </c>
+      <c r="B20">
+        <v>544624</v>
+      </c>
+      <c r="C20">
+        <v>567359</v>
+      </c>
+      <c r="D20">
+        <v>531882</v>
+      </c>
+      <c r="E20">
+        <v>428740</v>
+      </c>
+      <c r="F20">
+        <v>488338</v>
+      </c>
+      <c r="G20">
+        <v>492385</v>
+      </c>
+      <c r="H20">
+        <v>461893</v>
+      </c>
+      <c r="I20">
+        <v>499947</v>
+      </c>
+      <c r="J20">
+        <v>501625</v>
+      </c>
+      <c r="K20">
+        <v>514640</v>
+      </c>
+      <c r="L20">
+        <v>527515</v>
+      </c>
+      <c r="M20">
+        <v>495681</v>
+      </c>
+      <c r="N20">
+        <v>463245</v>
+      </c>
+      <c r="O20">
+        <v>439963</v>
+      </c>
+      <c r="P20">
+        <v>334198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43379</v>
+      </c>
+      <c r="B21">
+        <v>550121</v>
+      </c>
+      <c r="C21">
+        <v>559391</v>
+      </c>
+      <c r="D21">
+        <v>517916</v>
+      </c>
+      <c r="E21">
+        <v>500207</v>
+      </c>
+      <c r="F21">
+        <v>457180</v>
+      </c>
+      <c r="G21">
+        <v>408805</v>
+      </c>
+      <c r="H21">
+        <v>466821</v>
+      </c>
+      <c r="I21">
+        <v>457007</v>
+      </c>
+      <c r="J21">
+        <v>512275</v>
+      </c>
+      <c r="K21">
+        <v>508526</v>
+      </c>
+      <c r="L21">
+        <v>509489</v>
+      </c>
+      <c r="M21">
+        <v>532281</v>
+      </c>
+      <c r="N21">
+        <v>427646</v>
+      </c>
+      <c r="O21">
+        <v>377098</v>
+      </c>
+      <c r="P21">
+        <v>228966</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43386</v>
+      </c>
+      <c r="B22">
+        <v>554136</v>
+      </c>
+      <c r="C22">
+        <v>531779</v>
+      </c>
+      <c r="D22">
+        <v>560727</v>
+      </c>
+      <c r="E22">
+        <v>542629</v>
+      </c>
+      <c r="F22">
+        <v>538640</v>
+      </c>
+      <c r="G22">
+        <v>525483</v>
+      </c>
+      <c r="H22">
+        <v>511440</v>
+      </c>
+      <c r="I22">
+        <v>520428</v>
+      </c>
+      <c r="J22">
+        <v>421896</v>
+      </c>
+      <c r="K22">
+        <v>469040</v>
+      </c>
+      <c r="L22">
+        <v>511998</v>
+      </c>
+      <c r="M22">
+        <v>508960</v>
+      </c>
+      <c r="N22">
+        <v>526298</v>
+      </c>
+      <c r="O22">
+        <v>428496</v>
+      </c>
+      <c r="P22">
+        <v>370255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43407</v>
+      </c>
+      <c r="B23">
+        <v>562174</v>
+      </c>
+      <c r="C23">
+        <v>524590</v>
+      </c>
+      <c r="D23">
+        <v>517846</v>
+      </c>
+      <c r="E23">
+        <v>509697</v>
+      </c>
+      <c r="F23">
+        <v>499049</v>
+      </c>
+      <c r="G23">
+        <v>501116</v>
+      </c>
+      <c r="H23">
+        <v>496132</v>
+      </c>
+      <c r="I23">
+        <v>499626</v>
+      </c>
+      <c r="J23">
+        <v>454295</v>
+      </c>
+      <c r="K23">
+        <v>446816</v>
+      </c>
+      <c r="L23">
+        <v>497043</v>
+      </c>
+      <c r="M23">
+        <v>507719</v>
+      </c>
+      <c r="N23">
+        <v>506779</v>
+      </c>
+      <c r="O23">
+        <v>458367</v>
+      </c>
+      <c r="P23">
+        <v>373758</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43428</v>
+      </c>
+      <c r="B24">
+        <v>545360</v>
+      </c>
+      <c r="C24">
+        <v>537550</v>
+      </c>
+      <c r="D24">
+        <v>540913</v>
+      </c>
+      <c r="E24">
+        <v>531224</v>
+      </c>
+      <c r="F24">
+        <v>537123</v>
+      </c>
+      <c r="G24">
+        <v>548303</v>
+      </c>
+      <c r="H24">
+        <v>561075</v>
+      </c>
+      <c r="I24">
+        <v>551253</v>
+      </c>
+      <c r="J24">
+        <v>544580</v>
+      </c>
+      <c r="K24">
+        <v>444572</v>
+      </c>
+      <c r="L24">
+        <v>459999</v>
+      </c>
+      <c r="M24">
+        <v>541696</v>
+      </c>
+      <c r="N24">
+        <v>551636</v>
+      </c>
+      <c r="O24">
+        <v>464044</v>
+      </c>
+      <c r="P24">
+        <v>368516</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43715</v>
+      </c>
+      <c r="B25">
+        <v>457344</v>
+      </c>
+      <c r="C25">
+        <v>449662</v>
+      </c>
+      <c r="D25">
+        <v>438395</v>
+      </c>
+      <c r="E25">
+        <v>420464</v>
+      </c>
+      <c r="F25">
+        <v>410753</v>
+      </c>
+      <c r="G25">
+        <v>450686</v>
+      </c>
+      <c r="H25">
+        <v>466246</v>
+      </c>
+      <c r="I25">
+        <v>434481</v>
+      </c>
+      <c r="J25">
+        <v>367598</v>
+      </c>
+      <c r="K25">
+        <v>429469</v>
+      </c>
+      <c r="L25">
+        <v>478746</v>
+      </c>
+      <c r="M25">
+        <v>485188</v>
+      </c>
+      <c r="N25">
+        <v>460637</v>
+      </c>
+      <c r="O25">
+        <v>360452</v>
+      </c>
+      <c r="P25">
+        <v>330994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43729</v>
+      </c>
+      <c r="B26">
+        <v>439500</v>
+      </c>
+      <c r="C26">
+        <v>470712</v>
+      </c>
+      <c r="D26">
+        <v>444811</v>
+      </c>
+      <c r="E26">
+        <v>417644</v>
+      </c>
+      <c r="F26">
+        <v>395240</v>
+      </c>
+      <c r="G26">
+        <v>405731</v>
+      </c>
+      <c r="H26">
+        <v>437988</v>
+      </c>
+      <c r="I26">
+        <v>427825</v>
+      </c>
+      <c r="J26">
+        <v>434772</v>
+      </c>
+      <c r="K26">
+        <v>443056</v>
+      </c>
+      <c r="L26">
+        <v>450388</v>
+      </c>
+      <c r="M26">
+        <v>358443</v>
+      </c>
+      <c r="N26">
+        <v>393334</v>
+      </c>
+      <c r="O26">
+        <v>341731</v>
+      </c>
+      <c r="P26">
+        <v>314396</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43743</v>
+      </c>
+      <c r="B27">
+        <v>536872</v>
+      </c>
+      <c r="C27">
+        <v>506267</v>
+      </c>
+      <c r="D27">
+        <v>484903</v>
+      </c>
+      <c r="E27">
+        <v>495539</v>
+      </c>
+      <c r="F27">
+        <v>447455</v>
+      </c>
+      <c r="G27">
+        <v>429057</v>
+      </c>
+      <c r="H27">
+        <v>438316</v>
+      </c>
+      <c r="I27">
+        <v>450661</v>
+      </c>
+      <c r="J27">
+        <v>427281</v>
+      </c>
+      <c r="K27">
+        <v>419969</v>
+      </c>
+      <c r="L27">
+        <v>453741</v>
+      </c>
+      <c r="M27">
+        <v>460063</v>
+      </c>
+      <c r="N27">
+        <v>487930</v>
+      </c>
+      <c r="O27">
+        <v>395273</v>
+      </c>
+      <c r="P27">
+        <v>301231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43764</v>
+      </c>
+      <c r="B28">
+        <v>409732</v>
+      </c>
+      <c r="C28">
+        <v>345815</v>
+      </c>
+      <c r="D28">
+        <v>411769</v>
+      </c>
+      <c r="E28">
+        <v>236150</v>
+      </c>
+      <c r="F28">
+        <v>415084</v>
+      </c>
+      <c r="G28">
+        <v>418755</v>
+      </c>
+      <c r="H28">
+        <v>462783</v>
+      </c>
+      <c r="I28">
+        <v>422515</v>
+      </c>
+      <c r="J28">
+        <v>404615</v>
+      </c>
+      <c r="K28">
+        <v>441254</v>
+      </c>
+      <c r="L28">
+        <v>452255</v>
+      </c>
+      <c r="M28">
+        <v>473573</v>
+      </c>
+      <c r="N28">
+        <v>483869</v>
+      </c>
+      <c r="O28">
+        <v>392862</v>
+      </c>
+      <c r="P28">
+        <v>312192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43778</v>
+      </c>
+      <c r="B29">
+        <v>440007</v>
+      </c>
+      <c r="C29">
+        <v>463843</v>
+      </c>
+      <c r="D29">
+        <v>421522</v>
+      </c>
+      <c r="E29">
+        <v>424083</v>
+      </c>
+      <c r="F29">
+        <v>424328</v>
+      </c>
+      <c r="G29">
+        <v>424022</v>
+      </c>
+      <c r="H29">
+        <v>415927</v>
+      </c>
+      <c r="I29">
+        <v>410663</v>
+      </c>
+      <c r="J29">
+        <v>401631</v>
+      </c>
+      <c r="K29">
+        <v>436425</v>
+      </c>
+      <c r="L29">
+        <v>434925</v>
+      </c>
+      <c r="M29">
+        <v>473652</v>
+      </c>
+      <c r="N29">
+        <v>452337</v>
+      </c>
+      <c r="O29">
+        <v>383356</v>
+      </c>
+      <c r="P29">
+        <v>308833</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43792</v>
+      </c>
+      <c r="B30">
+        <v>446262</v>
+      </c>
+      <c r="C30">
+        <v>470641</v>
+      </c>
+      <c r="D30">
+        <v>426395</v>
+      </c>
+      <c r="E30">
+        <v>429374</v>
+      </c>
+      <c r="F30">
+        <v>466379</v>
+      </c>
+      <c r="G30">
+        <v>498136</v>
+      </c>
+      <c r="H30">
+        <v>493181</v>
+      </c>
+      <c r="I30">
+        <v>494340</v>
+      </c>
+      <c r="J30">
+        <v>431686</v>
+      </c>
+      <c r="K30">
+        <v>413523</v>
+      </c>
+      <c r="L30">
+        <v>430083</v>
+      </c>
+      <c r="M30">
+        <v>470380</v>
+      </c>
+      <c r="N30">
+        <v>486820</v>
+      </c>
+      <c r="O30">
+        <v>398060</v>
+      </c>
+      <c r="P30">
+        <v>336070</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE7F9FB-122C-49B0-B14B-F428CCFED8E6}">
   <dimension ref="A1:Y16"/>
   <sheetViews>
@@ -29599,7 +32275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCA92E9-F73E-4997-A8AA-C8273709BE10}">
   <dimension ref="A1:Y44"/>
   <sheetViews>
@@ -32973,7 +35649,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC3709-77B6-421E-B5D0-F9BC0815F8A0}">
   <dimension ref="A1:Y44"/>
   <sheetViews>
@@ -36347,7 +39023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF2F734B-C7D2-4779-AAE6-824E33DF8F1F}">
   <dimension ref="A1:J40"/>
   <sheetViews>
@@ -37197,7 +39873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E2E3D0-3DC2-4DB0-A7A4-1E7BFDD789B9}">
   <dimension ref="A1:I40"/>
   <sheetViews>
@@ -38028,12 +40704,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100AA540-0832-4110-933D-A2F4B5ECE0BA}">
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38921,7 +41597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E90E7C5-D6B5-4122-8A46-7038DC14E692}">
   <dimension ref="A1:X16"/>
   <sheetViews>
@@ -40116,1201 +42792,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B1A811-A38F-4335-A6D5-4CAA636AF908}">
-  <dimension ref="A1:X16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:X16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B1">
-        <v>5</v>
-      </c>
-      <c r="C1">
-        <v>10</v>
-      </c>
-      <c r="D1">
-        <v>15</v>
-      </c>
-      <c r="E1">
-        <v>20</v>
-      </c>
-      <c r="F1">
-        <v>25</v>
-      </c>
-      <c r="G1">
-        <v>30</v>
-      </c>
-      <c r="H1">
-        <v>35</v>
-      </c>
-      <c r="I1">
-        <v>40</v>
-      </c>
-      <c r="J1">
-        <v>45</v>
-      </c>
-      <c r="K1">
-        <v>50</v>
-      </c>
-      <c r="L1">
-        <v>55</v>
-      </c>
-      <c r="M1">
-        <v>60</v>
-      </c>
-      <c r="N1">
-        <v>65</v>
-      </c>
-      <c r="O1">
-        <v>70</v>
-      </c>
-      <c r="P1">
-        <v>75</v>
-      </c>
-      <c r="Q1">
-        <v>80</v>
-      </c>
-      <c r="R1">
-        <v>85</v>
-      </c>
-      <c r="S1">
-        <v>90</v>
-      </c>
-      <c r="T1">
-        <v>95</v>
-      </c>
-      <c r="U1">
-        <v>100</v>
-      </c>
-      <c r="V1">
-        <v>105</v>
-      </c>
-      <c r="W1">
-        <v>110</v>
-      </c>
-      <c r="X1">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>0.140725844167991</v>
-      </c>
-      <c r="C2">
-        <v>0.212302973502598</v>
-      </c>
-      <c r="D2">
-        <v>0.272598262664487</v>
-      </c>
-      <c r="E2">
-        <v>0.30479582516741099</v>
-      </c>
-      <c r="F2">
-        <v>0.34253357159967901</v>
-      </c>
-      <c r="G2">
-        <v>0.33930418480368901</v>
-      </c>
-      <c r="H2">
-        <v>0.38916358473037899</v>
-      </c>
-      <c r="I2">
-        <v>0.41153904484168002</v>
-      </c>
-      <c r="J2">
-        <v>0.41542395619811601</v>
-      </c>
-      <c r="K2">
-        <v>0.44649572059598303</v>
-      </c>
-      <c r="L2">
-        <v>0.45180277182537798</v>
-      </c>
-      <c r="M2">
-        <v>0.41449070115732001</v>
-      </c>
-      <c r="N2">
-        <v>0.39794823810114999</v>
-      </c>
-      <c r="O2">
-        <v>0.377327647297236</v>
-      </c>
-      <c r="P2">
-        <v>0.35432417513574699</v>
-      </c>
-      <c r="Q2">
-        <v>0.33712136370013102</v>
-      </c>
-      <c r="R2">
-        <v>0.329311506878532</v>
-      </c>
-      <c r="S2">
-        <v>0.307866107886271</v>
-      </c>
-      <c r="T2">
-        <v>0.28852491954231402</v>
-      </c>
-      <c r="U2">
-        <v>0.26562471516771402</v>
-      </c>
-      <c r="V2">
-        <v>0.24396939171720999</v>
-      </c>
-      <c r="W2">
-        <v>0.236286439777697</v>
-      </c>
-      <c r="X2">
-        <v>0.221827528065869</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>0.14131697569589599</v>
-      </c>
-      <c r="C3">
-        <v>0.20817032422720999</v>
-      </c>
-      <c r="D3">
-        <v>0.27888798377731899</v>
-      </c>
-      <c r="E3">
-        <v>0.33631633227076602</v>
-      </c>
-      <c r="F3">
-        <v>0.38546324692605899</v>
-      </c>
-      <c r="G3">
-        <v>0.38769878840011202</v>
-      </c>
-      <c r="H3">
-        <v>0.413248215302014</v>
-      </c>
-      <c r="I3">
-        <v>0.41100115474411197</v>
-      </c>
-      <c r="J3">
-        <v>0.43128436456631303</v>
-      </c>
-      <c r="K3">
-        <v>0.48877898652658203</v>
-      </c>
-      <c r="L3">
-        <v>0.50939998356440896</v>
-      </c>
-      <c r="M3">
-        <v>0.48818475713342302</v>
-      </c>
-      <c r="N3">
-        <v>0.484804739089778</v>
-      </c>
-      <c r="O3">
-        <v>0.47314007252006601</v>
-      </c>
-      <c r="P3">
-        <v>0.45857433864429797</v>
-      </c>
-      <c r="Q3">
-        <v>0.432059159452931</v>
-      </c>
-      <c r="R3">
-        <v>0.39996515593174797</v>
-      </c>
-      <c r="S3">
-        <v>0.35952088051961001</v>
-      </c>
-      <c r="T3">
-        <v>0.33358436747495201</v>
-      </c>
-      <c r="U3">
-        <v>0.30888273567408697</v>
-      </c>
-      <c r="V3">
-        <v>0.28835487743580202</v>
-      </c>
-      <c r="W3">
-        <v>0.27104563089142403</v>
-      </c>
-      <c r="X3">
-        <v>0.25033045908128898</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>0.13052543786488699</v>
-      </c>
-      <c r="C4">
-        <v>0.19656410951477299</v>
-      </c>
-      <c r="D4">
-        <v>0.30687878189359502</v>
-      </c>
-      <c r="E4">
-        <v>0.36927978745932999</v>
-      </c>
-      <c r="F4">
-        <v>0.37944924730086999</v>
-      </c>
-      <c r="G4">
-        <v>0.35942564312202502</v>
-      </c>
-      <c r="H4">
-        <v>0.41979896697872499</v>
-      </c>
-      <c r="I4">
-        <v>0.43426571761849198</v>
-      </c>
-      <c r="J4">
-        <v>0.43142948486478999</v>
-      </c>
-      <c r="K4">
-        <v>0.463558951841199</v>
-      </c>
-      <c r="L4">
-        <v>0.46235839580413501</v>
-      </c>
-      <c r="M4">
-        <v>0.43392205315356702</v>
-      </c>
-      <c r="N4">
-        <v>0.42900142694499699</v>
-      </c>
-      <c r="O4">
-        <v>0.42742206722127801</v>
-      </c>
-      <c r="P4">
-        <v>0.41441749295846803</v>
-      </c>
-      <c r="Q4">
-        <v>0.38478491112464502</v>
-      </c>
-      <c r="R4">
-        <v>0.360976037914089</v>
-      </c>
-      <c r="S4">
-        <v>0.33342078221223298</v>
-      </c>
-      <c r="T4">
-        <v>0.30483180409069099</v>
-      </c>
-      <c r="U4">
-        <v>0.28455875286571902</v>
-      </c>
-      <c r="V4">
-        <v>0.26385540892439402</v>
-      </c>
-      <c r="W4">
-        <v>0.25145687139359801</v>
-      </c>
-      <c r="X4">
-        <v>0.23575277024008001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>0.12864733849165599</v>
-      </c>
-      <c r="C5">
-        <v>0.24846250611503201</v>
-      </c>
-      <c r="D5">
-        <v>0.35474326630555703</v>
-      </c>
-      <c r="E5">
-        <v>0.37337889297882798</v>
-      </c>
-      <c r="F5">
-        <v>0.41114866850861198</v>
-      </c>
-      <c r="G5">
-        <v>0.40940229689756602</v>
-      </c>
-      <c r="H5">
-        <v>0.44525990306093899</v>
-      </c>
-      <c r="I5">
-        <v>0.48060087054404399</v>
-      </c>
-      <c r="J5">
-        <v>0.50544341978658702</v>
-      </c>
-      <c r="K5">
-        <v>0.54779823241094505</v>
-      </c>
-      <c r="L5">
-        <v>0.55146271257894497</v>
-      </c>
-      <c r="M5">
-        <v>0.522730286792503</v>
-      </c>
-      <c r="N5">
-        <v>0.496989448865226</v>
-      </c>
-      <c r="O5">
-        <v>0.480845224041835</v>
-      </c>
-      <c r="P5">
-        <v>0.45727943261614801</v>
-      </c>
-      <c r="Q5">
-        <v>0.426289508811031</v>
-      </c>
-      <c r="R5">
-        <v>0.40951059206265999</v>
-      </c>
-      <c r="S5">
-        <v>0.38278107085539498</v>
-      </c>
-      <c r="T5">
-        <v>0.35700528606952597</v>
-      </c>
-      <c r="U5">
-        <v>0.31832321933532498</v>
-      </c>
-      <c r="V5">
-        <v>0.29438428711319797</v>
-      </c>
-      <c r="W5">
-        <v>0.27563303283559099</v>
-      </c>
-      <c r="X5">
-        <v>0.25406489545389399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>9.0752804922186001E-2</v>
-      </c>
-      <c r="C6">
-        <v>0.21392734608024</v>
-      </c>
-      <c r="D6">
-        <v>0.35851407214451497</v>
-      </c>
-      <c r="E6">
-        <v>0.41562359087587197</v>
-      </c>
-      <c r="F6">
-        <v>0.45983042854927397</v>
-      </c>
-      <c r="G6">
-        <v>0.51327330439852303</v>
-      </c>
-      <c r="H6">
-        <v>0.56432651035171599</v>
-      </c>
-      <c r="I6">
-        <v>0.56289779845679799</v>
-      </c>
-      <c r="J6">
-        <v>0.58452075969704798</v>
-      </c>
-      <c r="K6">
-        <v>0.59141588341530504</v>
-      </c>
-      <c r="L6">
-        <v>0.59761929260859403</v>
-      </c>
-      <c r="M6">
-        <v>0.54986062239295597</v>
-      </c>
-      <c r="N6">
-        <v>0.553662140272563</v>
-      </c>
-      <c r="O6">
-        <v>0.53580561536985905</v>
-      </c>
-      <c r="P6">
-        <v>0.48704822667519199</v>
-      </c>
-      <c r="Q6">
-        <v>0.45029806083803497</v>
-      </c>
-      <c r="R6">
-        <v>0.43521839114732203</v>
-      </c>
-      <c r="S6">
-        <v>0.39829118383609402</v>
-      </c>
-      <c r="T6">
-        <v>0.357235066772851</v>
-      </c>
-      <c r="U6">
-        <v>0.31579591846254601</v>
-      </c>
-      <c r="V6">
-        <v>0.286295858317348</v>
-      </c>
-      <c r="W6">
-        <v>0.26818139993289503</v>
-      </c>
-      <c r="X6">
-        <v>0.25273696695806802</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>0.14879369300911799</v>
-      </c>
-      <c r="C7">
-        <v>0.29907445266327098</v>
-      </c>
-      <c r="D7">
-        <v>0.41457506361323099</v>
-      </c>
-      <c r="E7">
-        <v>0.44969622078055799</v>
-      </c>
-      <c r="F7">
-        <v>0.48309217960540801</v>
-      </c>
-      <c r="G7">
-        <v>0.461559065531644</v>
-      </c>
-      <c r="H7">
-        <v>0.51031859786015399</v>
-      </c>
-      <c r="I7">
-        <v>0.52296974128686102</v>
-      </c>
-      <c r="J7">
-        <v>0.54379386955306197</v>
-      </c>
-      <c r="K7">
-        <v>0.59001005788101102</v>
-      </c>
-      <c r="L7">
-        <v>0.59556008287816398</v>
-      </c>
-      <c r="M7">
-        <v>0.56976231126952404</v>
-      </c>
-      <c r="N7">
-        <v>0.54968926796902295</v>
-      </c>
-      <c r="O7">
-        <v>0.52159005853989904</v>
-      </c>
-      <c r="P7">
-        <v>0.50248184591143097</v>
-      </c>
-      <c r="Q7">
-        <v>0.4696102378973</v>
-      </c>
-      <c r="R7">
-        <v>0.46189632610766201</v>
-      </c>
-      <c r="S7">
-        <v>0.42794194233229099</v>
-      </c>
-      <c r="T7">
-        <v>0.39433530684426099</v>
-      </c>
-      <c r="U7">
-        <v>0.35732273671577403</v>
-      </c>
-      <c r="V7">
-        <v>0.32298956931045703</v>
-      </c>
-      <c r="W7">
-        <v>0.29953765941858801</v>
-      </c>
-      <c r="X7">
-        <v>0.279596310347276</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>0.13379690125070001</v>
-      </c>
-      <c r="C8">
-        <v>0.25905816388090402</v>
-      </c>
-      <c r="D8">
-        <v>0.39949400463344398</v>
-      </c>
-      <c r="E8">
-        <v>0.45745816640415998</v>
-      </c>
-      <c r="F8">
-        <v>0.46465964060864501</v>
-      </c>
-      <c r="G8">
-        <v>0.45991806398539697</v>
-      </c>
-      <c r="H8">
-        <v>0.48214861230345302</v>
-      </c>
-      <c r="I8">
-        <v>0.49676184578426902</v>
-      </c>
-      <c r="J8">
-        <v>0.49193614800185997</v>
-      </c>
-      <c r="K8">
-        <v>0.50279462966055</v>
-      </c>
-      <c r="L8">
-        <v>0.51791941381598405</v>
-      </c>
-      <c r="M8">
-        <v>0.47443264776543298</v>
-      </c>
-      <c r="N8">
-        <v>0.45377076440218</v>
-      </c>
-      <c r="O8">
-        <v>0.42579853209773599</v>
-      </c>
-      <c r="P8">
-        <v>0.40729591318403402</v>
-      </c>
-      <c r="Q8">
-        <v>0.36732145710453901</v>
-      </c>
-      <c r="R8">
-        <v>0.36000065854280899</v>
-      </c>
-      <c r="S8">
-        <v>0.33176274553083401</v>
-      </c>
-      <c r="T8">
-        <v>0.29563291098519101</v>
-      </c>
-      <c r="U8">
-        <v>0.25939272919395201</v>
-      </c>
-      <c r="V8">
-        <v>0.23604149140681599</v>
-      </c>
-      <c r="W8">
-        <v>0.21734477090837701</v>
-      </c>
-      <c r="X8">
-        <v>0.204199209921752</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>0.124647203072225</v>
-      </c>
-      <c r="C9">
-        <v>0.214850166865521</v>
-      </c>
-      <c r="D9">
-        <v>0.30632070045376097</v>
-      </c>
-      <c r="E9">
-        <v>0.35415738788760498</v>
-      </c>
-      <c r="F9">
-        <v>0.37172068883887999</v>
-      </c>
-      <c r="G9">
-        <v>0.35110170793412498</v>
-      </c>
-      <c r="H9">
-        <v>0.38993219283243802</v>
-      </c>
-      <c r="I9">
-        <v>0.40950334502225799</v>
-      </c>
-      <c r="J9">
-        <v>0.43161126151095403</v>
-      </c>
-      <c r="K9">
-        <v>0.44474389773003498</v>
-      </c>
-      <c r="L9">
-        <v>0.45315682634590898</v>
-      </c>
-      <c r="M9">
-        <v>0.437114215847974</v>
-      </c>
-      <c r="N9">
-        <v>0.431013380693758</v>
-      </c>
-      <c r="O9">
-        <v>0.417511169654811</v>
-      </c>
-      <c r="P9">
-        <v>0.39593724974019101</v>
-      </c>
-      <c r="Q9">
-        <v>0.37705356525880901</v>
-      </c>
-      <c r="R9">
-        <v>0.368745595241946</v>
-      </c>
-      <c r="S9">
-        <v>0.34968190525641202</v>
-      </c>
-      <c r="T9">
-        <v>0.327756606332051</v>
-      </c>
-      <c r="U9">
-        <v>0.30336549266139801</v>
-      </c>
-      <c r="V9">
-        <v>0.28552353892535398</v>
-      </c>
-      <c r="W9">
-        <v>0.26608755168501502</v>
-      </c>
-      <c r="X9">
-        <v>0.24595549675496101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>0.118118628359592</v>
-      </c>
-      <c r="C10">
-        <v>0.21693149531726799</v>
-      </c>
-      <c r="D10">
-        <v>0.29992041639605099</v>
-      </c>
-      <c r="E10">
-        <v>0.35233139963718202</v>
-      </c>
-      <c r="F10">
-        <v>0.38290810471254699</v>
-      </c>
-      <c r="G10">
-        <v>0.40671670803552701</v>
-      </c>
-      <c r="H10">
-        <v>0.45835177077716099</v>
-      </c>
-      <c r="I10">
-        <v>0.47130450335037199</v>
-      </c>
-      <c r="J10">
-        <v>0.48322476097109701</v>
-      </c>
-      <c r="K10">
-        <v>0.49913512470862897</v>
-      </c>
-      <c r="L10">
-        <v>0.51318161594704204</v>
-      </c>
-      <c r="M10">
-        <v>0.50166270414743597</v>
-      </c>
-      <c r="N10">
-        <v>0.49406051720008198</v>
-      </c>
-      <c r="O10">
-        <v>0.48126485949013798</v>
-      </c>
-      <c r="P10">
-        <v>0.448208601359672</v>
-      </c>
-      <c r="Q10">
-        <v>0.41346020822432999</v>
-      </c>
-      <c r="R10">
-        <v>0.40669196936798901</v>
-      </c>
-      <c r="S10">
-        <v>0.38858369153864403</v>
-      </c>
-      <c r="T10">
-        <v>0.36719345875529502</v>
-      </c>
-      <c r="U10">
-        <v>0.33775153968337601</v>
-      </c>
-      <c r="V10">
-        <v>0.30901792511592402</v>
-      </c>
-      <c r="W10">
-        <v>0.28732630409541299</v>
-      </c>
-      <c r="X10">
-        <v>0.27227040227252203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>0.10914508365803301</v>
-      </c>
-      <c r="C11">
-        <v>0.21328410725737901</v>
-      </c>
-      <c r="D11">
-        <v>0.28233604165731402</v>
-      </c>
-      <c r="E11">
-        <v>0.31554864762790102</v>
-      </c>
-      <c r="F11">
-        <v>0.35032310296607</v>
-      </c>
-      <c r="G11">
-        <v>0.34270727923467798</v>
-      </c>
-      <c r="H11">
-        <v>0.388267528414939</v>
-      </c>
-      <c r="I11">
-        <v>0.42467138828406797</v>
-      </c>
-      <c r="J11">
-        <v>0.43290888526667498</v>
-      </c>
-      <c r="K11">
-        <v>0.44459822553192202</v>
-      </c>
-      <c r="L11">
-        <v>0.45724306588180302</v>
-      </c>
-      <c r="M11">
-        <v>0.45965578738273699</v>
-      </c>
-      <c r="N11">
-        <v>0.43990694723485202</v>
-      </c>
-      <c r="O11">
-        <v>0.41230060067091201</v>
-      </c>
-      <c r="P11">
-        <v>0.38157988668385401</v>
-      </c>
-      <c r="Q11">
-        <v>0.35460810786786701</v>
-      </c>
-      <c r="R11">
-        <v>0.33926144322443602</v>
-      </c>
-      <c r="S11">
-        <v>0.321264220720475</v>
-      </c>
-      <c r="T11">
-        <v>0.304215986126808</v>
-      </c>
-      <c r="U11">
-        <v>0.28399275586109701</v>
-      </c>
-      <c r="V11">
-        <v>0.25740834989614803</v>
-      </c>
-      <c r="W11">
-        <v>0.24404128331428199</v>
-      </c>
-      <c r="X11">
-        <v>0.23071010281500501</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>18</v>
-      </c>
-      <c r="B12">
-        <v>0.119079587017917</v>
-      </c>
-      <c r="C12">
-        <v>0.22936052094062601</v>
-      </c>
-      <c r="D12">
-        <v>0.30951443099620402</v>
-      </c>
-      <c r="E12">
-        <v>0.37799876257384601</v>
-      </c>
-      <c r="F12">
-        <v>0.376261293058958</v>
-      </c>
-      <c r="G12">
-        <v>0.39224322252504101</v>
-      </c>
-      <c r="H12">
-        <v>0.438485072147695</v>
-      </c>
-      <c r="I12">
-        <v>0.45860428951742599</v>
-      </c>
-      <c r="J12">
-        <v>0.481395015255071</v>
-      </c>
-      <c r="K12">
-        <v>0.54322361430223698</v>
-      </c>
-      <c r="L12">
-        <v>0.58157074921859597</v>
-      </c>
-      <c r="M12">
-        <v>0.58834691124570704</v>
-      </c>
-      <c r="N12">
-        <v>0.56076295184508795</v>
-      </c>
-      <c r="O12">
-        <v>0.54126476175885196</v>
-      </c>
-      <c r="P12">
-        <v>0.51852648821539205</v>
-      </c>
-      <c r="Q12">
-        <v>0.495316422925416</v>
-      </c>
-      <c r="R12">
-        <v>0.47991602682080597</v>
-      </c>
-      <c r="S12">
-        <v>0.45229585998628602</v>
-      </c>
-      <c r="T12">
-        <v>0.42559761535458501</v>
-      </c>
-      <c r="U12">
-        <v>0.39765736537795598</v>
-      </c>
-      <c r="V12">
-        <v>0.37666748367104202</v>
-      </c>
-      <c r="W12">
-        <v>0.34776146430409099</v>
-      </c>
-      <c r="X12">
-        <v>0.31928974343370098</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>19</v>
-      </c>
-      <c r="B13">
-        <v>0.13999245069359201</v>
-      </c>
-      <c r="C13">
-        <v>0.27804790203493601</v>
-      </c>
-      <c r="D13">
-        <v>0.41648770947578301</v>
-      </c>
-      <c r="E13">
-        <v>0.49816124021177399</v>
-      </c>
-      <c r="F13">
-        <v>0.54195853675794203</v>
-      </c>
-      <c r="G13">
-        <v>0.52757047441209304</v>
-      </c>
-      <c r="H13">
-        <v>0.55860703484472196</v>
-      </c>
-      <c r="I13">
-        <v>0.60489072417654599</v>
-      </c>
-      <c r="J13">
-        <v>0.62502855677744695</v>
-      </c>
-      <c r="K13">
-        <v>0.64361679124924798</v>
-      </c>
-      <c r="L13">
-        <v>0.67052032404554796</v>
-      </c>
-      <c r="M13">
-        <v>0.66113544459001805</v>
-      </c>
-      <c r="N13">
-        <v>0.66771959912149503</v>
-      </c>
-      <c r="O13">
-        <v>0.66371940652919503</v>
-      </c>
-      <c r="P13">
-        <v>0.62664089155969604</v>
-      </c>
-      <c r="Q13">
-        <v>0.58011769203608199</v>
-      </c>
-      <c r="R13">
-        <v>0.53687067964981205</v>
-      </c>
-      <c r="S13">
-        <v>0.49171179320944902</v>
-      </c>
-      <c r="T13">
-        <v>0.43877968654559302</v>
-      </c>
-      <c r="U13">
-        <v>0.38615580376413799</v>
-      </c>
-      <c r="V13">
-        <v>0.338803399671121</v>
-      </c>
-      <c r="W13">
-        <v>0.30405087182381801</v>
-      </c>
-      <c r="X13">
-        <v>0.269312158912976</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>0.14984939759036101</v>
-      </c>
-      <c r="C14">
-        <v>0.322312523088289</v>
-      </c>
-      <c r="D14">
-        <v>0.55106145717174004</v>
-      </c>
-      <c r="E14">
-        <v>0.59659477355637602</v>
-      </c>
-      <c r="F14">
-        <v>0.61888611210281996</v>
-      </c>
-      <c r="G14">
-        <v>0.56883739529671895</v>
-      </c>
-      <c r="H14">
-        <v>0.58054739750251905</v>
-      </c>
-      <c r="I14">
-        <v>0.61745042616581702</v>
-      </c>
-      <c r="J14">
-        <v>0.63432475998438997</v>
-      </c>
-      <c r="K14">
-        <v>0.66346800862111099</v>
-      </c>
-      <c r="L14">
-        <v>0.69212337924781198</v>
-      </c>
-      <c r="M14">
-        <v>0.68674382453738003</v>
-      </c>
-      <c r="N14">
-        <v>0.68075908401072405</v>
-      </c>
-      <c r="O14">
-        <v>0.65734374442076304</v>
-      </c>
-      <c r="P14">
-        <v>0.62141264163852195</v>
-      </c>
-      <c r="Q14">
-        <v>0.57939985529323201</v>
-      </c>
-      <c r="R14">
-        <v>0.55379366977975897</v>
-      </c>
-      <c r="S14">
-        <v>0.52080201088586997</v>
-      </c>
-      <c r="T14">
-        <v>0.48230120228182999</v>
-      </c>
-      <c r="U14">
-        <v>0.437403312616024</v>
-      </c>
-      <c r="V14">
-        <v>0.39387206905152999</v>
-      </c>
-      <c r="W14">
-        <v>0.36553843447265599</v>
-      </c>
-      <c r="X14">
-        <v>0.32159028050715399</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>21</v>
-      </c>
-      <c r="B15">
-        <v>0.121665707157935</v>
-      </c>
-      <c r="C15">
-        <v>0.22660089282364801</v>
-      </c>
-      <c r="D15">
-        <v>0.36047685743135399</v>
-      </c>
-      <c r="E15">
-        <v>0.46741026490687299</v>
-      </c>
-      <c r="F15">
-        <v>0.51143095254183801</v>
-      </c>
-      <c r="G15">
-        <v>0.51685134344925998</v>
-      </c>
-      <c r="H15">
-        <v>0.53521973476654605</v>
-      </c>
-      <c r="I15">
-        <v>0.55529910480636302</v>
-      </c>
-      <c r="J15">
-        <v>0.53539335640265395</v>
-      </c>
-      <c r="K15">
-        <v>0.55205958002778299</v>
-      </c>
-      <c r="L15">
-        <v>0.54185046518918001</v>
-      </c>
-      <c r="M15">
-        <v>0.53687402343851798</v>
-      </c>
-      <c r="N15">
-        <v>0.54690083367748998</v>
-      </c>
-      <c r="O15">
-        <v>0.54191467179571595</v>
-      </c>
-      <c r="P15">
-        <v>0.519905705200571</v>
-      </c>
-      <c r="Q15">
-        <v>0.51353863396305</v>
-      </c>
-      <c r="R15">
-        <v>0.53082392874327</v>
-      </c>
-      <c r="S15">
-        <v>0.502136808206881</v>
-      </c>
-      <c r="T15">
-        <v>0.50401674794915696</v>
-      </c>
-      <c r="U15">
-        <v>0.49087591744575299</v>
-      </c>
-      <c r="V15">
-        <v>0.46277702157567202</v>
-      </c>
-      <c r="W15">
-        <v>0.44898297884332899</v>
-      </c>
-      <c r="X15">
-        <v>0.42748525840857599</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>22</v>
-      </c>
-      <c r="B16">
-        <v>7.9015103686076393E-2</v>
-      </c>
-      <c r="C16">
-        <v>0.15952376204056301</v>
-      </c>
-      <c r="D16">
-        <v>0.243544002718314</v>
-      </c>
-      <c r="E16">
-        <v>0.303172908985057</v>
-      </c>
-      <c r="F16">
-        <v>0.38112126886220898</v>
-      </c>
-      <c r="G16">
-        <v>0.34029427466577</v>
-      </c>
-      <c r="H16">
-        <v>0.396014545572347</v>
-      </c>
-      <c r="I16">
-        <v>0.437818262091349</v>
-      </c>
-      <c r="J16">
-        <v>0.460538177905292</v>
-      </c>
-      <c r="K16">
-        <v>0.49049991772370599</v>
-      </c>
-      <c r="L16">
-        <v>0.47195960881843402</v>
-      </c>
-      <c r="M16">
-        <v>0.45815209510234001</v>
-      </c>
-      <c r="N16">
-        <v>0.474015986704446</v>
-      </c>
-      <c r="O16">
-        <v>0.48624211694706498</v>
-      </c>
-      <c r="P16">
-        <v>0.49889641071583302</v>
-      </c>
-      <c r="Q16">
-        <v>0.51790871561978202</v>
-      </c>
-      <c r="R16">
-        <v>0.54773340072744203</v>
-      </c>
-      <c r="S16">
-        <v>0.53569552514948005</v>
-      </c>
-      <c r="T16">
-        <v>0.57072151652260705</v>
-      </c>
-      <c r="U16">
-        <v>0.59516043468475699</v>
-      </c>
-      <c r="V16">
-        <v>0.58147773609689102</v>
-      </c>
-      <c r="W16">
-        <v>0.56041075340945601</v>
-      </c>
-      <c r="X16">
-        <v>0.53511328224474397</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
New visualizations per Adam's comments
</commit_message>
<xml_diff>
--- a/ana/resilient.xlsx
+++ b/ana/resilient.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu.6544\Documents\GitHub\COTA-AccessibilityReliability\ana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CB1BAE-FD45-4DA9-B214-EC33C7A2BEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A4A3D9-0BC8-4B7F-89D5-0C2328A5206C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14175" firstSheet="1" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14175" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="date&amp;time" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
     <t>Home Game Days</t>
   </si>
   <si>
-    <t>C:\Users\liu.6544\Documents\GitHub\COTA-AccessibilityReliability\vis\resilience\three_days.tif</t>
+    <t>C:\Users\liu.6544\Documents\GitHub\COTA-AccessibilityReliability\vis\resilience\7pm.tif</t>
   </si>
 </sst>
 </file>
@@ -4621,7 +4621,7 @@
           <c:x val="8.6320816687098081E-2"/>
           <c:y val="4.4414556288572035E-2"/>
           <c:w val="0.89591217680931268"/>
-          <c:h val="0.65656011917429224"/>
+          <c:h val="0.76466822728240047"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -4755,8 +4755,212 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>peak_number!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Game Start Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>peak_number!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>43344</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43351</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43379</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43386</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43407</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43428</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43715</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43729</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43743</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43764</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43778</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43792</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>peak_number!$D$2:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1C23-49B3-9843-C3FD75332B0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>peak_number!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Game End Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>peak_number!$G$2:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>16.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.133333333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.166666666666666</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.866666666666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.033333333333335</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.016666666666666</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.583333333333334</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-910D-4EE2-8393-38B428EC0D7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>peak_number!$C$1</c:f>
@@ -4874,132 +5078,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1C23-49B3-9843-C3FD75332B0F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>peak_number!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Game Start Time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>peak_number!$A$2:$A$14</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>43344</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43351</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43365</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43379</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43386</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43407</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43428</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43715</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43729</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43743</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43764</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43778</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43792</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>peak_number!$D$2:$D$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1C23-49B3-9843-C3FD75332B0F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5052,8 +5130,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.89407888118476564"/>
-              <c:y val="0.69674398808257076"/>
+              <c:x val="0.89407885045404933"/>
+              <c:y val="0.90214939348797618"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -25723,7 +25801,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Game Start: 3:30 / 4:00 pm</a:t>
+              <a:t>Game Start: 15:30 / 16:00</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -26276,14 +26354,6 @@
             <a:r>
               <a:rPr lang="en-US" b="1"/>
               <a:t>Game Start: 12:00</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>pm</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -26798,13 +26868,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t>Game Start: 7:30</a:t>
+              <a:t>Game Start: 19:30</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> pm</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -39073,16 +39138,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1433510</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>433385</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>147635</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>576260</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -43126,8 +43191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97EC4F49-7FB8-4751-807F-3492689DAFAE}">
   <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P21"/>
+    <sheetView topLeftCell="U10" workbookViewId="0">
+      <selection activeCell="AV12" sqref="AV12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45526,7 +45591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05EBA4F-6466-4CB8-A00A-33172ED87E46}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
@@ -45937,63 +46002,63 @@
         <v>29</v>
       </c>
       <c r="B9" s="7">
-        <f>AVERAGE(B2:B7)</f>
+        <f t="shared" ref="B9:P9" si="0">AVERAGE(B2:B7)</f>
         <v>0.32594499999567622</v>
       </c>
       <c r="C9" s="7">
-        <f>AVERAGE(C2:C7)</f>
+        <f t="shared" si="0"/>
         <v>0.35143877877103852</v>
       </c>
       <c r="D9" s="7">
-        <f>AVERAGE(D2:D7)</f>
+        <f t="shared" si="0"/>
         <v>0.35120281291420835</v>
       </c>
       <c r="E9" s="7">
-        <f>AVERAGE(E2:E7)</f>
+        <f t="shared" si="0"/>
         <v>0.36895664415873952</v>
       </c>
       <c r="F9" s="7">
-        <f>AVERAGE(F2:F7)</f>
+        <f t="shared" si="0"/>
         <v>0.39689434535875595</v>
       </c>
       <c r="G9" s="7">
-        <f>AVERAGE(G2:G7)</f>
+        <f t="shared" si="0"/>
         <v>0.41366301418023038</v>
       </c>
       <c r="H9" s="7">
-        <f>AVERAGE(H2:H7)</f>
+        <f t="shared" si="0"/>
         <v>0.39746141539531976</v>
       </c>
       <c r="I9" s="7">
-        <f>AVERAGE(I2:I7)</f>
+        <f t="shared" si="0"/>
         <v>0.42477478920818251</v>
       </c>
       <c r="J9" s="7">
-        <f>AVERAGE(J2:J7)</f>
+        <f t="shared" si="0"/>
         <v>0.44374391276800607</v>
       </c>
       <c r="K9" s="7">
-        <f>AVERAGE(K2:K7)</f>
+        <f t="shared" si="0"/>
         <v>0.47388828753751538</v>
       </c>
       <c r="L9" s="7">
-        <f>AVERAGE(L2:L7)</f>
+        <f t="shared" si="0"/>
         <v>0.43748421728572667</v>
       </c>
       <c r="M9" s="7">
-        <f>AVERAGE(M2:M7)</f>
+        <f t="shared" si="0"/>
         <v>0.39875294058662192</v>
       </c>
       <c r="N9" s="7">
-        <f>AVERAGE(N2:N7)</f>
+        <f t="shared" si="0"/>
         <v>0.40952961315098441</v>
       </c>
       <c r="O9" s="7">
-        <f>AVERAGE(O2:O7)</f>
+        <f t="shared" si="0"/>
         <v>0.37624113862310482</v>
       </c>
       <c r="P9" s="7">
-        <f>AVERAGE(P2:P7)</f>
+        <f t="shared" si="0"/>
         <v>0.37294226711854583</v>
       </c>
     </row>
@@ -46057,7 +46122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1172EF6C-D4A3-4EB6-8D73-298C079FEF54}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:P6"/>
     </sheetView>
   </sheetViews>
@@ -46324,7 +46389,7 @@
         <v>0.31554925485511726</v>
       </c>
       <c r="C6" s="6">
-        <f t="shared" ref="C6:P8" si="0">AVERAGE(C2:C5)</f>
+        <f t="shared" ref="C6:P6" si="0">AVERAGE(C2:C5)</f>
         <v>0.29960094437363999</v>
       </c>
       <c r="D6" s="6">

</xml_diff>